<commit_message>
organización de ekyword en test cases y steps, iteración con binding y cucumber
</commit_message>
<xml_diff>
--- a/Data Files/DD_DigitalCertificate.xlsx
+++ b/Data Files/DD_DigitalCertificate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lope112166\Katalon Studio\PT\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lope112166\Katalon Studio\katalonbasic\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>XLS_Usuario</t>
   </si>
@@ -42,9 +42,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>XLS_PersonType</t>
-  </si>
-  <si>
     <t>XLS_Identification</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
   </si>
   <si>
     <t>XLS_PostalCode</t>
-  </si>
-  <si>
-    <t>Natural</t>
   </si>
   <si>
     <t>Pepito</t>
@@ -422,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,71 +436,104 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
       </c>
       <c r="H2">
         <v>1234567890</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2">
+        <v>110012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="J2">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>1234567890</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3">
         <v>110012</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>